<commit_message>
Add group work agreement to timetable
</commit_message>
<xml_diff>
--- a/book/Supporting/Timetable.xlsx
+++ b/book/Supporting/Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbartlett/Documents/git_repos/RM1_Resources/book/Supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EC23DE-56F9-EF4A-8A19-30F5B49480AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C2E0AD-19D5-3C4E-8C13-FF61D99BB424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FEC2AC94-DE11-4304-8C62-67F1F3B88347}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{FEC2AC94-DE11-4304-8C62-67F1F3B88347}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Week</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Discussion 2</t>
+  </si>
+  <si>
+    <t>Formative: Group work agreement</t>
   </si>
 </sst>
 </file>
@@ -564,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186DAC8A-208F-48D2-A2B0-EF358B1AE4DE}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -608,7 +611,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>45187</v>
+        <v>45180</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -619,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>45194</v>
+        <v>45187</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -639,7 +642,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>45201</v>
+        <v>45194</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -659,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>45208</v>
+        <v>45201</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -672,6 +675,9 @@
       </c>
       <c r="F5" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -679,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>45215</v>
+        <v>45208</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -699,7 +705,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>45222</v>
+        <v>45215</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -722,7 +728,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>45229</v>
+        <v>45222</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -736,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>45236</v>
+        <v>45229</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -759,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -782,7 +788,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>45250</v>
+        <v>45243</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -802,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>45257</v>
+        <v>45250</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -825,7 +831,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>45264</v>
+        <v>45257</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -836,7 +842,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>45271</v>
+        <v>45264</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -844,6 +850,9 @@
       <c r="G14" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update timetable for lab titles
</commit_message>
<xml_diff>
--- a/book/Supporting/Timetable.xlsx
+++ b/book/Supporting/Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbartlett/Documents/git_repos/RM1_Resources/book/Supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C2E0AD-19D5-3C4E-8C13-FF61D99BB424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBEB347-F4DD-9548-8387-0B4312C8B92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{FEC2AC94-DE11-4304-8C62-67F1F3B88347}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FEC2AC94-DE11-4304-8C62-67F1F3B88347}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Assessment</t>
   </si>
   <si>
-    <t>Week Commencing</t>
-  </si>
-  <si>
     <t>Inductions</t>
   </si>
   <si>
@@ -176,31 +173,34 @@
     <t>Data skills 2</t>
   </si>
   <si>
-    <t>Introduction 1</t>
-  </si>
-  <si>
-    <t>Introduction 2</t>
-  </si>
-  <si>
-    <t>Method 1</t>
-  </si>
-  <si>
-    <t>Method 2</t>
-  </si>
-  <si>
-    <t>Results 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results 2 </t>
-  </si>
-  <si>
-    <t>Discussion 1</t>
-  </si>
-  <si>
-    <t>Discussion 2</t>
-  </si>
-  <si>
     <t>Formative: Group work agreement</t>
+  </si>
+  <si>
+    <t>Finding and reading journal articles</t>
+  </si>
+  <si>
+    <t>Introduction structure</t>
+  </si>
+  <si>
+    <t>Academic writing</t>
+  </si>
+  <si>
+    <t>Method structure</t>
+  </si>
+  <si>
+    <t>Communicating correlation results</t>
+  </si>
+  <si>
+    <t>Communicating t-test results</t>
+  </si>
+  <si>
+    <t>Discussion structure</t>
+  </si>
+  <si>
+    <t>Abstract structure</t>
+  </si>
+  <si>
+    <t>W/C</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -614,7 +614,7 @@
         <v>45180</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -625,16 +625,16 @@
         <v>45187</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -645,16 +645,16 @@
         <v>45194</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -665,19 +665,19 @@
         <v>45201</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -688,16 +688,16 @@
         <v>45208</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -708,19 +708,19 @@
         <v>45215</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -731,10 +731,10 @@
         <v>45222</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -745,19 +745,19 @@
         <v>45229</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -768,19 +768,19 @@
         <v>45236</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -791,16 +791,16 @@
         <v>45243</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -811,19 +811,19 @@
         <v>45250</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -834,7 +834,7 @@
         <v>45257</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -845,10 +845,10 @@
         <v>45264</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Rerender book to check progress
</commit_message>
<xml_diff>
--- a/book/Supporting/Timetable.xlsx
+++ b/book/Supporting/Timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbartlett/Documents/git_repos/RM1_Resources/book/Supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBEB347-F4DD-9548-8387-0B4312C8B92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E8FBF5-2E45-9A40-9382-2BD86C630749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FEC2AC94-DE11-4304-8C62-67F1F3B88347}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edit timetable and link to stage one report in group agreement
</commit_message>
<xml_diff>
--- a/book/Supporting/Timetable.xlsx
+++ b/book/Supporting/Timetable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbartlett/Documents/git_repos/RM1_Resources/book/Supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E8FBF5-2E45-9A40-9382-2BD86C630749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57D73AC-4426-6B4B-9116-0FF6699EEAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FEC2AC94-DE11-4304-8C62-67F1F3B88347}"/>
   </bookViews>
@@ -124,43 +124,10 @@
     <t>* Chapter 12 - Screening data</t>
   </si>
   <si>
-    <t>* Quantitative Project / MSLQ Overview</t>
-  </si>
-  <si>
-    <t>* Types of evidence and finding sources
-* RQs and hypotheses</t>
-  </si>
-  <si>
-    <t>* APA referencing
-* Academic writing</t>
-  </si>
-  <si>
-    <t>* Introductions
-* Rationale</t>
-  </si>
-  <si>
-    <t>* RQ and hypotheses Padlet
-* Stage one template</t>
-  </si>
-  <si>
-    <t>* Method section</t>
-  </si>
-  <si>
-    <t>* Results section</t>
-  </si>
-  <si>
-    <t>* Plagirism 
-* Ethics</t>
-  </si>
-  <si>
     <t>* Chapter 10 - t-tests
 * Chapter 11 - Power and effect sizes</t>
   </si>
   <si>
-    <t>* Discussion section
-* Abstracts</t>
-  </si>
-  <si>
     <t>MCQ</t>
   </si>
   <si>
@@ -201,6 +168,39 @@
   </si>
   <si>
     <t>W/C</t>
+  </si>
+  <si>
+    <t>* Registered report and MSLQ overview</t>
+  </si>
+  <si>
+    <t>* Finding, reading, and organising journal articles
+* Group work agreement</t>
+  </si>
+  <si>
+    <t>* Introduction structure
+* Identifying the rationale</t>
+  </si>
+  <si>
+    <t>* Scientific writing
+* Paragraph structure
+* Citation placement</t>
+  </si>
+  <si>
+    <t>* Method structure
+* Researcher degrees of freedom</t>
+  </si>
+  <si>
+    <t>* Correlation results sections
+* Reporting power analyses</t>
+  </si>
+  <si>
+    <t>* t-test results sections</t>
+  </si>
+  <si>
+    <t>* Discussion structure</t>
+  </si>
+  <si>
+    <t>* Abstract structure</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -634,10 +634,10 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -648,13 +648,13 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -668,19 +668,19 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -691,13 +691,13 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -711,16 +711,16 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -748,16 +748,16 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -771,19 +771,19 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -794,16 +794,16 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -814,16 +814,16 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Correct stage 2 AIS and overview formatting
</commit_message>
<xml_diff>
--- a/book/Supporting/Timetable.xlsx
+++ b/book/Supporting/Timetable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/james_bartlett_glasgow_ac_uk/Documents/Documents/repos/RM1_Resources/book/Supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{A57D73AC-4426-6B4B-9116-0FF6699EEAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20725B58-B709-4753-BEDE-1513C312DCCA}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{A57D73AC-4426-6B4B-9116-0FF6699EEAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB525C2C-3553-4E26-840F-95D4780D5723}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FEC2AC94-DE11-4304-8C62-67F1F3B88347}"/>
   </bookViews>
@@ -172,11 +172,6 @@
 * Identifying the rationale</t>
   </si>
   <si>
-    <t>* Scientific writing
-* Paragraph structure
-* Citation placement</t>
-  </si>
-  <si>
     <t>* Method structure
 * Researcher degrees of freedom</t>
   </si>
@@ -201,6 +196,9 @@
   </si>
   <si>
     <t>Decision making in data analysis</t>
+  </si>
+  <si>
+    <t>* Scientific writing, Paragraph structure, Citation placement</t>
   </si>
 </sst>
 </file>
@@ -570,7 +568,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +578,7 @@
     <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -680,7 +678,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -697,7 +695,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -717,7 +715,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -745,7 +743,7 @@
         <v>45229</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
@@ -754,7 +752,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
         <v>27</v>
@@ -768,7 +766,7 @@
         <v>45236</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>36</v>
@@ -777,7 +775,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
         <v>28</v>
@@ -800,7 +798,7 @@
         <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -811,7 +809,7 @@
         <v>45250</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
@@ -820,7 +818,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
         <v>29</v>

</xml_diff>